<commit_message>
Vergleich hinzugefügt und Sachen umgezogen, die nicht mehr existent sind oder nicht mehr verwendet werden.
</commit_message>
<xml_diff>
--- a/Rosenholz.View/Combinations_F22.xlsx
+++ b/Rosenholz.View/Combinations_F22.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://siemens-my.sharepoint.com/personal/frederic_arnolin_siemens_com/Documents/src/VisualStudio/Rosenholz/Rosenholz/Rosenholz.View/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\OneDrive - Siemens AG\src\VisualStudio\Rosenholz\Rosenholz\Rosenholz.View\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{67E23803-9736-4F4A-870C-3D6E4B3E4397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D18C1896-FBB4-4099-A79F-C8E561DA3261}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80805B54-BBBA-47E7-AB9C-B0680EDC5058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57490" yWindow="6430" windowWidth="29020" windowHeight="17770" xr2:uid="{C8A52FCD-43D2-4FAF-B396-0191536B3089}"/>
+    <workbookView xWindow="57490" yWindow="6430" windowWidth="29020" windowHeight="17770" activeTab="1" xr2:uid="{C8A52FCD-43D2-4FAF-B396-0191536B3089}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="F16F22-Referenz" sheetId="1" r:id="rId1"/>
+    <sheet name="AU-Referenz" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="16">
   <si>
     <t>YEAR</t>
   </si>
@@ -77,6 +78,12 @@
   </si>
   <si>
     <t>ex</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -241,6 +248,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,17 +272,200 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="168">
+  <dxfs count="195">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1758,8 +1954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D87F9FB-85D3-4C65-BD8D-C1B7BBC95576}">
   <dimension ref="A2:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:A56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1801,7 +1997,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -1829,16 +2025,16 @@
       <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="10">
+      <c r="N4" s="8"/>
+      <c r="O4" s="7">
         <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -1855,18 +2051,18 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="10"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="12"/>
+      <c r="A6" s="5"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1894,16 +2090,16 @@
       <c r="K7" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="7"/>
-      <c r="O7" s="10" t="s">
+      <c r="N7" s="11"/>
+      <c r="O7" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -1920,18 +2116,18 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="10"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="12"/>
+      <c r="A9" s="5"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1959,16 +2155,16 @@
       <c r="K10" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="M10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="10">
+      <c r="N10" s="8"/>
+      <c r="O10" s="7">
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -1985,18 +2181,18 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="10"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="12"/>
+      <c r="A12" s="5"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="12"/>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -2024,16 +2220,16 @@
       <c r="K13" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="M13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="7"/>
-      <c r="O13" s="10" t="s">
+      <c r="N13" s="11"/>
+      <c r="O13" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
+      <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -2050,18 +2246,18 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="10"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="12"/>
+      <c r="A15" s="5"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -2089,16 +2285,16 @@
       <c r="K16" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="M16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="7"/>
-      <c r="O16" s="10" t="s">
+      <c r="N16" s="11"/>
+      <c r="O16" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="12"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -2115,18 +2311,18 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="10"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="7"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
+      <c r="A18" s="5"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19" s="12"/>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -2154,16 +2350,16 @@
       <c r="K19" t="s">
         <v>11</v>
       </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4" t="s">
+      <c r="M19" s="8"/>
+      <c r="N19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O19" s="10">
+      <c r="O19" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20" s="12"/>
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
         <v>6</v>
       </c>
@@ -2180,18 +2376,18 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="10"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="7"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
+      <c r="A21" s="5"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A22" s="12"/>
+      <c r="A22" s="5"/>
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -2219,16 +2415,16 @@
       <c r="K22" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N22" s="7"/>
-      <c r="O22" s="10" t="s">
+      <c r="N22" s="11"/>
+      <c r="O22" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23" s="12"/>
+      <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>6</v>
       </c>
@@ -2245,18 +2441,18 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="10"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="7"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24" s="12"/>
+      <c r="A24" s="5"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25" s="12"/>
+      <c r="A25" s="5"/>
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -2284,16 +2480,16 @@
       <c r="K25" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4" t="s">
+      <c r="M25" s="8"/>
+      <c r="N25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O25" s="10">
+      <c r="O25" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
+      <c r="A26" s="5"/>
       <c r="B26" t="s">
         <v>6</v>
       </c>
@@ -2310,9 +2506,9 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="10"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C27" s="3"/>
@@ -2320,7 +2516,7 @@
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A28" s="11"/>
+      <c r="A28" s="4"/>
       <c r="B28" t="s">
         <v>7</v>
       </c>
@@ -2348,16 +2544,16 @@
       <c r="K28" t="s">
         <v>11</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="M28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N28" s="4"/>
-      <c r="O28" s="10">
+      <c r="N28" s="8"/>
+      <c r="O28" s="7">
         <v>-1</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A29" s="11"/>
+      <c r="A29" s="4"/>
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -2374,18 +2570,18 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="10"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="7"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A30" s="11"/>
+      <c r="A30" s="4"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A31" s="11"/>
+      <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>7</v>
       </c>
@@ -2413,16 +2609,16 @@
       <c r="K31" t="s">
         <v>11</v>
       </c>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4" t="s">
+      <c r="M31" s="8"/>
+      <c r="N31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O31" s="10">
+      <c r="O31" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A32" s="11"/>
+      <c r="A32" s="4"/>
       <c r="B32" t="s">
         <v>6</v>
       </c>
@@ -2439,18 +2635,18 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="10"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="7"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A33" s="11"/>
+      <c r="A33" s="4"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A34" s="11"/>
+      <c r="A34" s="4"/>
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -2478,16 +2674,16 @@
       <c r="K34" t="s">
         <v>11</v>
       </c>
-      <c r="M34" s="4" t="s">
+      <c r="M34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N34" s="4"/>
-      <c r="O34" s="10">
+      <c r="N34" s="8"/>
+      <c r="O34" s="7">
         <v>-1</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A35" s="11"/>
+      <c r="A35" s="4"/>
       <c r="B35" t="s">
         <v>6</v>
       </c>
@@ -2504,18 +2700,18 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="10"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="7"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A36" s="11"/>
+      <c r="A36" s="4"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
+      <c r="A37" s="4"/>
       <c r="B37" t="s">
         <v>7</v>
       </c>
@@ -2543,16 +2739,16 @@
       <c r="K37" t="s">
         <v>11</v>
       </c>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4" t="s">
+      <c r="M37" s="8"/>
+      <c r="N37" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O37" s="10">
+      <c r="O37" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A38" s="11"/>
+      <c r="A38" s="4"/>
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -2569,9 +2765,9 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="10"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="7"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C39" s="3"/>
@@ -2579,7 +2775,7 @@
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
+      <c r="A40" s="6"/>
       <c r="B40" t="s">
         <v>7</v>
       </c>
@@ -2607,16 +2803,16 @@
       <c r="K40" t="s">
         <v>11</v>
       </c>
-      <c r="M40" s="4" t="s">
+      <c r="M40" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N40" s="4"/>
-      <c r="O40" s="10">
+      <c r="N40" s="8"/>
+      <c r="O40" s="7">
         <v>-1</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
+      <c r="A41" s="6"/>
       <c r="B41" t="s">
         <v>6</v>
       </c>
@@ -2633,18 +2829,18 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="10"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="7"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
+      <c r="A42" s="6"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
+      <c r="A43" s="6"/>
       <c r="B43" t="s">
         <v>7</v>
       </c>
@@ -2672,16 +2868,16 @@
       <c r="K43" t="s">
         <v>11</v>
       </c>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4" t="s">
+      <c r="M43" s="8"/>
+      <c r="N43" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O43" s="10">
+      <c r="O43" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A44" s="13"/>
+      <c r="A44" s="6"/>
       <c r="B44" t="s">
         <v>6</v>
       </c>
@@ -2698,18 +2894,18 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="10"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="7"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
+      <c r="A45" s="6"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A46" s="13"/>
+      <c r="A46" s="6"/>
       <c r="B46" t="s">
         <v>7</v>
       </c>
@@ -2737,16 +2933,16 @@
       <c r="K46" t="s">
         <v>11</v>
       </c>
-      <c r="M46" s="4" t="s">
+      <c r="M46" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N46" s="4"/>
-      <c r="O46" s="10">
+      <c r="N46" s="8"/>
+      <c r="O46" s="7">
         <v>-1</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A47" s="13"/>
+      <c r="A47" s="6"/>
       <c r="B47" t="s">
         <v>6</v>
       </c>
@@ -2763,18 +2959,18 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="10"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="7"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A48" s="13"/>
+      <c r="A48" s="6"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A49" s="13"/>
+      <c r="A49" s="6"/>
       <c r="B49" t="s">
         <v>7</v>
       </c>
@@ -2802,16 +2998,16 @@
       <c r="K49" t="s">
         <v>11</v>
       </c>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4" t="s">
+      <c r="M49" s="8"/>
+      <c r="N49" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O49" s="10">
+      <c r="O49" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A50" s="13"/>
+      <c r="A50" s="6"/>
       <c r="B50" t="s">
         <v>6</v>
       </c>
@@ -2828,9 +3024,9 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="K50" s="2"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="10"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="7"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C51" s="3"/>
@@ -2866,11 +3062,11 @@
       <c r="K52" t="s">
         <v>11</v>
       </c>
-      <c r="M52" s="4" t="s">
+      <c r="M52" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N52" s="4"/>
-      <c r="O52" s="10">
+      <c r="N52" s="8"/>
+      <c r="O52" s="7">
         <v>-1</v>
       </c>
     </row>
@@ -2892,9 +3088,9 @@
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="K53" s="2"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="10"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="7"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
@@ -2931,11 +3127,11 @@
       <c r="K55" t="s">
         <v>11</v>
       </c>
-      <c r="M55" s="4"/>
-      <c r="N55" s="4" t="s">
+      <c r="M55" s="8"/>
+      <c r="N55" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O55" s="10">
+      <c r="O55" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2957,34 +3153,21 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="K56" s="2"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="10"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="O49:O50"/>
-    <mergeCell ref="O52:O53"/>
-    <mergeCell ref="O55:O56"/>
-    <mergeCell ref="O37:O38"/>
-    <mergeCell ref="O40:O41"/>
-    <mergeCell ref="O43:O44"/>
-    <mergeCell ref="O46:O47"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="O31:O32"/>
-    <mergeCell ref="O34:O35"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="N49:N50"/>
-    <mergeCell ref="M52:M53"/>
-    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="M13:N14"/>
+    <mergeCell ref="M16:N17"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="M7:N8"/>
     <mergeCell ref="M55:M56"/>
     <mergeCell ref="N55:N56"/>
     <mergeCell ref="M40:M41"/>
@@ -2993,6 +3176,11 @@
     <mergeCell ref="N43:N44"/>
     <mergeCell ref="M46:M47"/>
     <mergeCell ref="N46:N47"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="N49:N50"/>
+    <mergeCell ref="M52:M53"/>
+    <mergeCell ref="N52:N53"/>
     <mergeCell ref="M31:M32"/>
     <mergeCell ref="N31:N32"/>
     <mergeCell ref="M34:M35"/>
@@ -3004,630 +3192,1226 @@
     <mergeCell ref="M28:M29"/>
     <mergeCell ref="N28:N29"/>
     <mergeCell ref="M22:N23"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="M13:N14"/>
-    <mergeCell ref="M16:N17"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="O31:O32"/>
+    <mergeCell ref="O34:O35"/>
+    <mergeCell ref="O49:O50"/>
+    <mergeCell ref="O52:O53"/>
+    <mergeCell ref="O55:O56"/>
+    <mergeCell ref="O37:O38"/>
+    <mergeCell ref="O40:O41"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="O46:O47"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K6 G3:K3 G9:K9 G12:K12 G15:K15 G27:K27 G30:K30 G33:K33 G36:K36 G39:K39 G51:K51 G57:K368">
-    <cfRule type="containsText" dxfId="167" priority="166" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="194" priority="166" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="167" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="193" priority="167" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="165" priority="168" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="192" priority="168" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:K5">
-    <cfRule type="containsText" dxfId="164" priority="163" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="191" priority="163" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="164" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="190" priority="164" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="162" priority="165" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="189" priority="165" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:K7 J8">
-    <cfRule type="containsText" dxfId="161" priority="160" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="188" priority="160" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="161" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="187" priority="161" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="162" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="186" priority="162" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:K10 J11">
-    <cfRule type="containsText" dxfId="158" priority="157" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="185" priority="157" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="157" priority="158" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="184" priority="158" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="156" priority="159" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="183" priority="159" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:K13 J14">
-    <cfRule type="containsText" dxfId="155" priority="154" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="182" priority="154" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="154" priority="155" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="181" priority="155" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="156" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="180" priority="156" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:K18 G21:K21 G24:K24">
-    <cfRule type="containsText" dxfId="152" priority="151" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="179" priority="151" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="152" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="178" priority="152" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="150" priority="153" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="177" priority="153" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16:K16 J17">
-    <cfRule type="containsText" dxfId="149" priority="148" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="176" priority="148" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="149" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="175" priority="149" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="147" priority="150" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="174" priority="150" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19:K19 J20">
-    <cfRule type="containsText" dxfId="146" priority="145" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="173" priority="145" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="146" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="172" priority="146" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="147" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="171" priority="147" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:K22 J23">
-    <cfRule type="containsText" dxfId="143" priority="142" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="170" priority="142" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="143" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="169" priority="143" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="144" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="168" priority="144" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25:K25 J26">
-    <cfRule type="containsText" dxfId="140" priority="139" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="167" priority="139" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="140" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="166" priority="140" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G25)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="141" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="165" priority="141" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:K28 J29">
-    <cfRule type="containsText" dxfId="137" priority="136" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="164" priority="136" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="137" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="163" priority="137" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="138" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="162" priority="138" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:K31 J32">
-    <cfRule type="containsText" dxfId="134" priority="133" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="161" priority="133" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="134" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="160" priority="134" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="135" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="159" priority="135" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34:K34 J35">
-    <cfRule type="containsText" dxfId="131" priority="130" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="158" priority="130" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="131" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="157" priority="131" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="132" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="156" priority="132" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:K37 J38">
-    <cfRule type="containsText" dxfId="128" priority="127" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="155" priority="127" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="128" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="154" priority="128" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="129" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="153" priority="129" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G42:K42 G45:K45 G48:K48">
-    <cfRule type="containsText" dxfId="125" priority="124" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="152" priority="124" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="125" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="151" priority="125" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G42)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="150" priority="126" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:K40 J41">
-    <cfRule type="containsText" dxfId="122" priority="121" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="149" priority="121" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="122" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="148" priority="122" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="147" priority="123" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43:K43 J44">
-    <cfRule type="containsText" dxfId="119" priority="118" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="146" priority="118" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="145" priority="119" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G43)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="144" priority="120" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46:K46 J47">
-    <cfRule type="containsText" dxfId="116" priority="115" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="143" priority="115" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="142" priority="116" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="141" priority="117" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49:K49 J50">
-    <cfRule type="containsText" dxfId="113" priority="112" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="140" priority="112" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="139" priority="113" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="138" priority="114" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54:K54">
-    <cfRule type="containsText" dxfId="110" priority="109" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="137" priority="109" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="136" priority="110" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="135" priority="111" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52:K52 J53">
-    <cfRule type="containsText" dxfId="107" priority="106" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="134" priority="106" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="133" priority="107" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="132" priority="108" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G55:K55 J56">
-    <cfRule type="containsText" dxfId="104" priority="103" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="131" priority="103" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="130" priority="104" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="129" priority="105" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:I8">
-    <cfRule type="containsText" dxfId="101" priority="100" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="128" priority="100" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="127" priority="101" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="126" priority="102" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:I11">
-    <cfRule type="containsText" dxfId="98" priority="97" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="125" priority="97" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="124" priority="98" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="123" priority="99" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:I14">
-    <cfRule type="containsText" dxfId="95" priority="94" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="122" priority="94" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="121" priority="95" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="96" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="120" priority="96" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:I17">
-    <cfRule type="containsText" dxfId="92" priority="91" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="119" priority="91" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="118" priority="92" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="93" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="117" priority="93" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:I20">
-    <cfRule type="containsText" dxfId="89" priority="88" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="116" priority="88" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="115" priority="89" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="114" priority="90" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:I23">
-    <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="113" priority="85" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="112" priority="86" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="87" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="111" priority="87" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26:I26">
-    <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="110" priority="82" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="109" priority="83" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="108" priority="84" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:I29">
-    <cfRule type="containsText" dxfId="80" priority="79" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="107" priority="79" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="106" priority="80" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="81" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="105" priority="81" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:I32">
-    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="104" priority="76" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="103" priority="77" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="102" priority="78" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35:I35">
-    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="101" priority="73" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="100" priority="74" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="75" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="99" priority="75" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38:I38">
-    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="98" priority="70" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="97" priority="71" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G38)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="96" priority="72" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G41:I41">
-    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="95" priority="67" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="94" priority="68" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="93" priority="69" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44:I44">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="92" priority="64" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="91" priority="65" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G44)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="66" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="90" priority="66" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:I47">
-    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="89" priority="61" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="88" priority="62" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="87" priority="63" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50:I50">
-    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="86" priority="58" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="85" priority="59" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="84" priority="60" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G53:I53">
-    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="83" priority="55" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="82" priority="56" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G53)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="81" priority="57" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56:I56">
-    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="80" priority="52" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",G56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="79" priority="53" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",G56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="78" priority="54" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",G56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="77" priority="49" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="76" priority="50" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="75" priority="51" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="74" priority="46" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="73" priority="47" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="72" priority="48" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="71" priority="43" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="70" priority="44" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="45" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="69" priority="45" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",K14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="68" priority="40" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="67" priority="41" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="66" priority="42" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",K17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="65" priority="37" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="64" priority="38" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="63" priority="39" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="62" priority="34" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="61" priority="35" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="60" priority="36" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",K23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="59" priority="31" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="58" priority="32" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K26)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="33" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="57" priority="33" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",K26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="56" priority="28" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",K29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="55" priority="29" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",K29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="NULL">
+    <cfRule type="containsText" dxfId="54" priority="30" operator="containsText" text="NULL">
       <formula>NOT(ISERROR(SEARCH("NULL",K29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
+    <cfRule type="containsText" dxfId="53" priority="25" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="26" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="27" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K35">
+    <cfRule type="containsText" dxfId="50" priority="22" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="23" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K35)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="24" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K38">
+    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K38)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K41">
+    <cfRule type="containsText" dxfId="44" priority="16" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="17" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K41)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="18" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K44">
+    <cfRule type="containsText" dxfId="41" priority="13" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="14" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K44)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="15" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K47">
+    <cfRule type="containsText" dxfId="38" priority="10" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="11" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="12" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K50">
+    <cfRule type="containsText" dxfId="35" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K50)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="9" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K53">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K53)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K56">
+    <cfRule type="containsText" dxfId="29" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",K56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",K56)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="NULL">
+      <formula>NOT(ISERROR(SEARCH("NULL",K56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <customProperties>
+    <customPr name="IbpWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5622F5F5-465E-4B0A-A8A1-0B5996DC1D6C}">
+  <dimension ref="B5:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" t="str">
+        <f>IF((C6&lt;C7),"TRUE",IF((C6&gt;C7),"FALSE","NULL"))</f>
+        <v>TRUE</v>
+      </c>
+      <c r="G6" t="str">
+        <f>IF((D6&lt;D7),"TRUE",IF((D6&gt;D7),"FALSE","NULL"))</f>
+        <v>TRUE</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" t="str">
+        <f>IF((C9&lt;C10),"TRUE",IF((C9&gt;C10),"FALSE","NULL"))</f>
+        <v>TRUE</v>
+      </c>
+      <c r="G9" t="str">
+        <f>IF((D9&lt;D10),"TRUE",IF((D9&gt;D10),"FALSE","NULL"))</f>
+        <v>FALSE</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="7"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="F12" t="str">
+        <f>IF((C12&lt;C13),"TRUE",IF((C12&gt;C13),"FALSE","NULL"))</f>
+        <v>TRUE</v>
+      </c>
+      <c r="G12" t="str">
+        <f>IF((D12&lt;D13),"TRUE",IF((D12&gt;D13),"FALSE","NULL"))</f>
+        <v>NULL</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="8"/>
+      <c r="M12" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3">
+        <v>23</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>23</v>
+      </c>
+      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="F15" t="str">
+        <f>IF((C15&lt;C16),"TRUE",IF((C15&gt;C16),"FALSE","NULL"))</f>
+        <v>FALSE</v>
+      </c>
+      <c r="G15" t="str">
+        <f>IF((D15&lt;D16),"TRUE",IF((D15&gt;D16),"FALSE","NULL"))</f>
+        <v>TRUE</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3">
+        <v>23</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="F18" t="str">
+        <f>IF((C18&lt;C19),"TRUE",IF((C18&gt;C19),"FALSE","NULL"))</f>
+        <v>FALSE</v>
+      </c>
+      <c r="G18" t="str">
+        <f>IF((D18&lt;D19),"TRUE",IF((D18&gt;D19),"FALSE","NULL"))</f>
+        <v>FALSE</v>
+      </c>
+      <c r="I18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="7"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3">
+        <v>23</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="F21" t="str">
+        <f>IF((C21&lt;C22),"TRUE",IF((C21&gt;C22),"FALSE","NULL"))</f>
+        <v>FALSE</v>
+      </c>
+      <c r="G21" t="str">
+        <f>IF((D21&lt;D22),"TRUE",IF((D21&gt;D22),"FALSE","NULL"))</f>
+        <v>NULL</v>
+      </c>
+      <c r="I21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3">
+        <v>22</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="7"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="F24" t="str">
+        <f>IF((C24&lt;C25),"TRUE",IF((C24&gt;C25),"FALSE","NULL"))</f>
+        <v>NULL</v>
+      </c>
+      <c r="G24" t="str">
+        <f>IF((D24&lt;D25),"TRUE",IF((D24&gt;D25),"FALSE","NULL"))</f>
+        <v>TRUE</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24" s="8"/>
+      <c r="M24" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="3">
+        <v>22</v>
+      </c>
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="7"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3">
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>3</v>
+      </c>
+      <c r="F27" t="str">
+        <f>IF((C27&lt;C28),"TRUE",IF((C27&gt;C28),"FALSE","NULL"))</f>
+        <v>NULL</v>
+      </c>
+      <c r="G27" t="str">
+        <f>IF((D27&lt;D28),"TRUE",IF((D27&gt;D28),"FALSE","NULL"))</f>
+        <v>FALSE</v>
+      </c>
+      <c r="I27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="3">
+        <v>22</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="3">
+        <v>22</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="F30" t="str">
+        <f>IF((C30&lt;C31),"TRUE",IF((C30&gt;C31),"FALSE","NULL"))</f>
+        <v>NULL</v>
+      </c>
+      <c r="G30" t="str">
+        <f>IF((D30&lt;D31),"TRUE",IF((D30&gt;D31),"FALSE","NULL"))</f>
+        <v>NULL</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L30" s="8"/>
+      <c r="M30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="3">
+        <v>22</v>
+      </c>
+      <c r="D31" s="3">
+        <v>2</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F6:I7">
     <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K32)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F6)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K32)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F6)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K35">
+      <formula>NOT(ISERROR(SEARCH("NULL",F6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9:I10">
     <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K38">
+      <formula>NOT(ISERROR(SEARCH("NULL",F9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12:I13">
     <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F12)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K38)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F12)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K41">
+      <formula>NOT(ISERROR(SEARCH("NULL",F12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15:I16">
     <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K41)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F15)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K44">
+      <formula>NOT(ISERROR(SEARCH("NULL",F15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:I19">
     <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K44)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K44)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K47">
+      <formula>NOT(ISERROR(SEARCH("NULL",F18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:I22">
     <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F21)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K50">
+      <formula>NOT(ISERROR(SEARCH("NULL",F21)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24:I25">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K50)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K50)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F24)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K53">
+      <formula>NOT(ISERROR(SEARCH("NULL",F24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27:I28">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F27)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F27)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K56">
+      <formula>NOT(ISERROR(SEARCH("NULL",F27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30:I31">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",K56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F30)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",K56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F30)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NULL">
-      <formula>NOT(ISERROR(SEARCH("NULL",K56)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NULL",F30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>